<commit_message>
Modificado: CUENTA_FINTECH.xlsx, añadido columna cliente_id
Para la relación cuenta-cliente
</commit_message>
<xml_diff>
--- a/Datos/CUENTA_FINTECH.xlsx
+++ b/Datos/CUENTA_FINTECH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97ECDF34-CD87-4CD8-9E1E-0C24027212DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E611B1-AEEF-4CF0-A501-C36647D45840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>estado</t>
   </si>
@@ -74,14 +74,25 @@
   </si>
   <si>
     <t>BAJA</t>
+  </si>
+  <si>
+    <t>cliente_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,9 +120,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FBF252-AA62-4344-9439-A520D3B46077}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +453,7 @@
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -460,8 +472,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -474,8 +489,11 @@
       <c r="D2" s="1">
         <v>44084</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -491,8 +509,11 @@
       <c r="E3" s="1">
         <v>42370</v>
       </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -505,8 +526,11 @@
       <c r="D4" s="1">
         <v>39588</v>
       </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -519,8 +543,11 @@
       <c r="D5" s="1">
         <v>43785</v>
       </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -533,8 +560,13 @@
       <c r="D6" s="1">
         <v>41311</v>
       </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/AngelSergioSM/ABD"
This reverts commit 9b13ab77744df04b22db569bcc065afa7da03e8e, reversing
changes made to d7626600e074263858753ed65e0d89d002e0be7d.
</commit_message>
<xml_diff>
--- a/Datos/CUENTA_FINTECH.xlsx
+++ b/Datos/CUENTA_FINTECH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A802D1-D915-4CA5-AF8B-2E42DAAE15EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E611B1-AEEF-4CF0-A501-C36647D45840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'main' of https://github.com/AngelSergioSM/ABD""
This reverts commit fd530ab3e840975b47946749fe3c24edd912812b.
</commit_message>
<xml_diff>
--- a/Datos/CUENTA_FINTECH.xlsx
+++ b/Datos/CUENTA_FINTECH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\ABD\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E611B1-AEEF-4CF0-A501-C36647D45840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A802D1-D915-4CA5-AF8B-2E42DAAE15EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel y nivel fisico modificados ya deberian funcionar todos
</commit_message>
<xml_diff>
--- a/Datos/CUENTA_FINTECH.xlsx
+++ b/Datos/CUENTA_FINTECH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A802D1-D915-4CA5-AF8B-2E42DAAE15EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2BB1BA-7B16-4204-B815-65769D92BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>estado</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>clasificacion</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>IBAN</t>
@@ -438,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FBF252-AA62-4344-9439-A520D3B46077}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,112 +455,97 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44084</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42353</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42370</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>39588</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44084</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1">
-        <v>42353</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42370</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>39588</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43785</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43785</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1">
         <v>41311</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>5</v>
       </c>
       <c r="I6" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios en los datos
</commit_message>
<xml_diff>
--- a/Datos/CUENTA_FINTECH.xlsx
+++ b/Datos/CUENTA_FINTECH.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ABD\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2BB1BA-7B16-4204-B815-65769D92BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A9D34-ACEF-4B46-AFA7-5A26A3C44957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>estado</t>
   </si>
@@ -52,12 +51,6 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>ES32 4434 344 34434</t>
-  </si>
-  <si>
-    <t>ES32 1226 347 77987</t>
-  </si>
-  <si>
     <t>ES32 5829 354  1000</t>
   </si>
   <si>
@@ -70,16 +63,19 @@
     <t>ALTA</t>
   </si>
   <si>
-    <t>BAJA</t>
-  </si>
-  <si>
     <t>cliente_id</t>
+  </si>
+  <si>
+    <t>POOLED</t>
+  </si>
+  <si>
+    <t>SEGREGADA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,23 +430,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FBF252-AA62-4344-9439-A520D3B46077}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -467,84 +463,64 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>39588</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44084</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43785</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1">
-        <v>42353</v>
-      </c>
-      <c r="D3" s="1">
-        <v>42370</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>39588</v>
+        <v>41311</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43785</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>41311</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G12" s="2"/>
     </row>
   </sheetData>

</xml_diff>